<commit_message>
split data into training set & testing set
</commit_message>
<xml_diff>
--- a/Marriage_Divorce_DB.xlsx
+++ b/Marriage_Divorce_DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Analytics\Divorce probability\Divorce-probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9359A60-A22D-4478-AD6D-516159603218}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F0648A-542D-431D-B62A-1E9CE78C4563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -956,41 +956,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.111632623</v>
       </c>
@@ -1180,7 +1182,7 @@
         <v>2.7601897900000001</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3.3553841549999999</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>1.962978994</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6.5273650419999996</v>
       </c>
@@ -1370,7 +1372,7 @@
         <v>2.858802802</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.2030749309999997</v>
       </c>
@@ -1465,7 +1467,7 @@
         <v>1.404620695</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6.8649618390000002</v>
       </c>
@@ -1560,7 +1562,7 @@
         <v>1.3188188810000001</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6.0724157050000001</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>2.3295120200000001</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5.6857693339999997</v>
       </c>
@@ -1750,7 +1752,7 @@
         <v>1.3925208440000001</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4.7742041119999996</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>2.4887219389999999</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9.3266523370000005</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>2.9496959270000001</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.2797018470000001</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>1.248016901</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.9464983600000001</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>2.0390560080000002</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3.845625955</v>
       </c>
@@ -2225,7 +2227,7 @@
         <v>2.1614495310000001</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3.8274650669999999</v>
       </c>
@@ -2320,7 +2322,7 @@
         <v>1.372262678</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9.0216478710000008</v>
       </c>
@@ -2415,7 +2417,7 @@
         <v>1.8458143549999999</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9.7334941609999994</v>
       </c>
@@ -2510,7 +2512,7 @@
         <v>2.2514304200000002</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.2860704189999996</v>
       </c>
@@ -2605,7 +2607,7 @@
         <v>2.4805538970000001</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5.8572489540000001</v>
       </c>
@@ -2700,7 +2702,7 @@
         <v>2.9159777629999999</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8.4807769129999997</v>
       </c>
@@ -2795,7 +2797,7 @@
         <v>1.898964595</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6.7623258699999997</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>2.0805847559999999</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.65068330699999999</v>
       </c>
@@ -2985,7 +2987,7 @@
         <v>1.619024317</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6.8976012569999998</v>
       </c>
@@ -3080,7 +3082,7 @@
         <v>2.0423842319999999</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.9256628689999999</v>
       </c>
@@ -3175,7 +3177,7 @@
         <v>2.7267339750000001</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.6938431129999998</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>2.1089700979999999</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2.0821102339999999</v>
       </c>
@@ -3365,7 +3367,7 @@
         <v>2.0948807810000001</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8.7887906699999991</v>
       </c>
@@ -3460,7 +3462,7 @@
         <v>2.8252259839999998</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7.0251619730000003</v>
       </c>
@@ -3555,7 +3557,7 @@
         <v>2.9304554500000002</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3.033132331</v>
       </c>
@@ -3650,7 +3652,7 @@
         <v>2.3294003860000001</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.3351747749999996</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>2.625045262</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6.3778817050000001</v>
       </c>
@@ -3840,7 +3842,7 @@
         <v>2.231843451</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9.3240597570000006</v>
       </c>
@@ -3935,7 +3937,7 @@
         <v>1.7063024899999999</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4.1114792969999998</v>
       </c>
@@ -4030,7 +4032,7 @@
         <v>2.4541173010000001</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4.6775323740000001</v>
       </c>
@@ -4125,7 +4127,7 @@
         <v>1.262316972</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8.0758233770000007</v>
       </c>
@@ -4220,7 +4222,7 @@
         <v>1.0330875719999999</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3.1496640509999998</v>
       </c>
@@ -4315,7 +4317,7 @@
         <v>2.526625514</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8.4768317900000003</v>
       </c>
@@ -4410,7 +4412,7 @@
         <v>2.8134789160000002</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2.1503743740000001</v>
       </c>
@@ -4505,7 +4507,7 @@
         <v>1.685199892</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3.199320744</v>
       </c>
@@ -4600,7 +4602,7 @@
         <v>1.827233058</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3.073316471</v>
       </c>
@@ -4695,7 +4697,7 @@
         <v>2.018697623</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5.6577042549999996</v>
       </c>
@@ -4790,7 +4792,7 @@
         <v>2.807019903</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1.8552671110000001</v>
       </c>
@@ -4885,7 +4887,7 @@
         <v>2.9401997049999999</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6.2193832999999996</v>
       </c>
@@ -4980,7 +4982,7 @@
         <v>2.7283910929999999</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1.457066864</v>
       </c>
@@ -5075,7 +5077,7 @@
         <v>2.3791588560000001</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3.8720651479999999</v>
       </c>
@@ -5170,7 +5172,7 @@
         <v>2.1568684060000001</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4.2496791189999996</v>
       </c>
@@ -5265,7 +5267,7 @@
         <v>2.0892454539999998</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5.2956371649999996</v>
       </c>
@@ -5360,7 +5362,7 @@
         <v>2.3755008769999999</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4.8775723949999996</v>
       </c>
@@ -5455,7 +5457,7 @@
         <v>1.042003528</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7.505987459</v>
       </c>
@@ -5550,7 +5552,7 @@
         <v>1.3393168419999999</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.5700638839999996</v>
       </c>
@@ -5645,7 +5647,7 @@
         <v>1.4937617729999999</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2.6521949779999998</v>
       </c>
@@ -5740,7 +5742,7 @@
         <v>2.615962675</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4.8056272450000002</v>
       </c>
@@ -5835,7 +5837,7 @@
         <v>1.9591760680000001</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2.0394573920000001</v>
       </c>
@@ -5930,7 +5932,7 @@
         <v>1.463561702</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9.0434956579999994</v>
       </c>
@@ -6025,7 +6027,7 @@
         <v>2.7185746819999999</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6.3275655530000003</v>
       </c>
@@ -6120,7 +6122,7 @@
         <v>2.4981472149999999</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9.5729682530000009</v>
       </c>
@@ -6215,7 +6217,7 @@
         <v>2.3321907369999999</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9.7138195970000005</v>
       </c>
@@ -6310,7 +6312,7 @@
         <v>2.8482328379999999</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3.1541557409999998</v>
       </c>
@@ -6405,7 +6407,7 @@
         <v>1.909519958</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.75838512700000005</v>
       </c>
@@ -6500,7 +6502,7 @@
         <v>1.461410232</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1.3355725540000001</v>
       </c>
@@ -6595,7 +6597,7 @@
         <v>1.296263293</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6.13628032</v>
       </c>
@@ -6690,7 +6692,7 @@
         <v>2.8225503619999999</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4.0695782070000002</v>
       </c>
@@ -6785,7 +6787,7 @@
         <v>2.3253798589999999</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2.7805801520000002</v>
       </c>
@@ -6880,7 +6882,7 @@
         <v>2.2282915650000001</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3.363461934</v>
       </c>
@@ -6975,7 +6977,7 @@
         <v>2.019971924</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.184739758</v>
       </c>
@@ -7070,7 +7072,7 @@
         <v>1.3126554619999999</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5.0455600220000001</v>
       </c>
@@ -7165,7 +7167,7 @@
         <v>1.5331706430000001</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3.6435125639999999</v>
       </c>
@@ -7260,7 +7262,7 @@
         <v>1.357002735</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9.1364504439999994</v>
       </c>
@@ -7355,7 +7357,7 @@
         <v>1.7193570869999999</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3.2249549439999998</v>
       </c>
@@ -7450,7 +7452,7 @@
         <v>1.062269245</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4.065189438</v>
       </c>
@@ -7545,7 +7547,7 @@
         <v>1.773216916</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.6005174650000003</v>
       </c>
@@ -7640,7 +7642,7 @@
         <v>1.880240726</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4.6338642610000003</v>
       </c>
@@ -7735,7 +7737,7 @@
         <v>1.867603259</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3.7998510990000001</v>
       </c>
@@ -7830,7 +7832,7 @@
         <v>2.53292121</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2.6523271689999999</v>
       </c>
@@ -7925,7 +7927,7 @@
         <v>2.6864838610000001</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5.9776249650000004</v>
       </c>
@@ -8020,7 +8022,7 @@
         <v>1.6568642659999999</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5.4378850569999999</v>
       </c>
@@ -8115,7 +8117,7 @@
         <v>2.5857880940000002</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2.2395502490000001</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v>1.384282056</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5.9483985260000001</v>
       </c>
@@ -8305,7 +8307,7 @@
         <v>2.3972216180000001</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>6.5094367540000002</v>
       </c>
@@ -8400,7 +8402,7 @@
         <v>1.3468634049999999</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.188713624</v>
       </c>
@@ -8495,7 +8497,7 @@
         <v>2.6126391280000001</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>7.0900558910000004</v>
       </c>
@@ -8590,7 +8592,7 @@
         <v>2.0766644520000002</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>6.4079026700000004</v>
       </c>
@@ -8685,7 +8687,7 @@
         <v>2.8817951960000001</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>3.336195306</v>
       </c>
@@ -8780,7 +8782,7 @@
         <v>2.3437898580000001</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>8.8567343009999995</v>
       </c>
@@ -8875,7 +8877,7 @@
         <v>2.9900396410000001</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2.788791056</v>
       </c>
@@ -8970,7 +8972,7 @@
         <v>2.5793418680000002</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>8.2939452679999999</v>
       </c>
@@ -9065,7 +9067,7 @@
         <v>1.3291437749999999</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5.0636886839999997</v>
       </c>
@@ -9160,7 +9162,7 @@
         <v>1.024549851</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4.7386238690000004</v>
       </c>
@@ -9255,7 +9257,7 @@
         <v>1.7816536860000001</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>8.1508628939999994</v>
       </c>
@@ -9350,7 +9352,7 @@
         <v>2.5716341329999999</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.62883908899999996</v>
       </c>
@@ -9445,7 +9447,7 @@
         <v>1.6443633559999999</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>3.2863320279999999</v>
       </c>
@@ -9540,7 +9542,7 @@
         <v>2.085356472</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2.0466708179999999</v>
       </c>
@@ -9635,7 +9637,7 @@
         <v>2.7889603360000002</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3.559281661</v>
       </c>
@@ -9730,7 +9732,7 @@
         <v>1.7908478219999999</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>9.5802410550000001</v>
       </c>
@@ -9825,7 +9827,7 @@
         <v>1.545559232</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>6.0010199990000004</v>
       </c>
@@ -9920,7 +9922,7 @@
         <v>1.0102146940000001</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7.073224851</v>
       </c>
@@ -10015,7 +10017,7 @@
         <v>1.8142555279999999</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1.9725029249999999</v>
       </c>
@@ -10110,7 +10112,7 @@
         <v>2.8754229790000001</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>6.9629868909999999</v>
       </c>
@@ -10205,7 +10207,7 @@
         <v>1.508493791</v>
       </c>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0.78244517800000002</v>
       </c>
@@ -10300,7 +10302,7 @@
         <v>1.56450248</v>
       </c>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>4.1814222819999998</v>
       </c>
@@ -10395,7 +10397,7 @@
         <v>2.6456534679999999</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3.487982514</v>
       </c>
@@ -10490,7 +10492,7 @@
         <v>1.75419788</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5.81875666</v>
       </c>

</xml_diff>

<commit_message>
found out correl between income & dP
</commit_message>
<xml_diff>
--- a/Marriage_Divorce_DB.xlsx
+++ b/Marriage_Divorce_DB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Analytics\Divorce probability\Divorce-probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F0648A-542D-431D-B62A-1E9CE78C4563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDD2740-5386-4490-A169-6257B2B340D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,28 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
-    <t>Age Gap</t>
-  </si>
-  <si>
     <t>Education</t>
-  </si>
-  <si>
-    <t>Economic Similarity</t>
-  </si>
-  <si>
-    <t>Social Similarities</t>
-  </si>
-  <si>
-    <t>Cultural Similarities</t>
-  </si>
-  <si>
-    <t>Social Gap</t>
-  </si>
-  <si>
-    <t>Common Interests</t>
-  </si>
-  <si>
-    <t>Religion Compatibility</t>
   </si>
   <si>
     <t>No of Children from Previous Marriage</t>
@@ -91,15 +70,6 @@
     <t>Loyalty</t>
   </si>
   <si>
-    <t>Height Ratio</t>
-  </si>
-  <si>
-    <t>Good Income</t>
-  </si>
-  <si>
-    <t>Self Confidence</t>
-  </si>
-  <si>
     <t>Relation with Non-spouse Before Marriage</t>
   </si>
   <si>
@@ -113,6 +83,36 @@
   </si>
   <si>
     <t>Divorce_Probability</t>
+  </si>
+  <si>
+    <t>Economic_Similarity</t>
+  </si>
+  <si>
+    <t>Social_Similarities</t>
+  </si>
+  <si>
+    <t>Cultural_Similarities</t>
+  </si>
+  <si>
+    <t>Social_Gap</t>
+  </si>
+  <si>
+    <t>Common_Interests</t>
+  </si>
+  <si>
+    <t>Religion_Compatibility</t>
+  </si>
+  <si>
+    <t>Good_Income</t>
+  </si>
+  <si>
+    <t>Height_Ratio</t>
+  </si>
+  <si>
+    <t>Self_Confidence</t>
+  </si>
+  <si>
+    <t>Age_Gap</t>
   </si>
 </sst>
 </file>
@@ -956,138 +956,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.111632623</v>
       </c>
@@ -1182,7 +1180,7 @@
         <v>2.7601897900000001</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3.3553841549999999</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>1.962978994</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6.5273650419999996</v>
       </c>
@@ -1372,7 +1370,7 @@
         <v>2.858802802</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5.2030749309999997</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>1.404620695</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6.8649618390000002</v>
       </c>
@@ -1562,7 +1560,7 @@
         <v>1.3188188810000001</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6.0724157050000001</v>
       </c>
@@ -1657,7 +1655,7 @@
         <v>2.3295120200000001</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5.6857693339999997</v>
       </c>
@@ -1752,7 +1750,7 @@
         <v>1.3925208440000001</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4.7742041119999996</v>
       </c>
@@ -1847,7 +1845,7 @@
         <v>2.4887219389999999</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9.3266523370000005</v>
       </c>
@@ -1942,7 +1940,7 @@
         <v>2.9496959270000001</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9.2797018470000001</v>
       </c>
@@ -2037,7 +2035,7 @@
         <v>1.248016901</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2.9464983600000001</v>
       </c>
@@ -2132,7 +2130,7 @@
         <v>2.0390560080000002</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3.845625955</v>
       </c>
@@ -2227,7 +2225,7 @@
         <v>2.1614495310000001</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3.8274650669999999</v>
       </c>
@@ -2322,7 +2320,7 @@
         <v>1.372262678</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9.0216478710000008</v>
       </c>
@@ -2417,7 +2415,7 @@
         <v>1.8458143549999999</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9.7334941609999994</v>
       </c>
@@ -2512,7 +2510,7 @@
         <v>2.2514304200000002</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7.2860704189999996</v>
       </c>
@@ -2607,7 +2605,7 @@
         <v>2.4805538970000001</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5.8572489540000001</v>
       </c>
@@ -2702,7 +2700,7 @@
         <v>2.9159777629999999</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8.4807769129999997</v>
       </c>
@@ -2797,7 +2795,7 @@
         <v>1.898964595</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6.7623258699999997</v>
       </c>
@@ -2892,7 +2890,7 @@
         <v>2.0805847559999999</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.65068330699999999</v>
       </c>
@@ -2987,7 +2985,7 @@
         <v>1.619024317</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6.8976012569999998</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>2.0423842319999999</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6.9256628689999999</v>
       </c>
@@ -3177,7 +3175,7 @@
         <v>2.7267339750000001</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2.6938431129999998</v>
       </c>
@@ -3272,7 +3270,7 @@
         <v>2.1089700979999999</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2.0821102339999999</v>
       </c>
@@ -3367,7 +3365,7 @@
         <v>2.0948807810000001</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8.7887906699999991</v>
       </c>
@@ -3462,7 +3460,7 @@
         <v>2.8252259839999998</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7.0251619730000003</v>
       </c>
@@ -3557,7 +3555,7 @@
         <v>2.9304554500000002</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3.033132331</v>
       </c>
@@ -3652,7 +3650,7 @@
         <v>2.3294003860000001</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7.3351747749999996</v>
       </c>
@@ -3747,7 +3745,7 @@
         <v>2.625045262</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6.3778817050000001</v>
       </c>
@@ -3842,7 +3840,7 @@
         <v>2.231843451</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9.3240597570000006</v>
       </c>
@@ -3937,7 +3935,7 @@
         <v>1.7063024899999999</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4.1114792969999998</v>
       </c>
@@ -4032,7 +4030,7 @@
         <v>2.4541173010000001</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4.6775323740000001</v>
       </c>
@@ -4127,7 +4125,7 @@
         <v>1.262316972</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8.0758233770000007</v>
       </c>
@@ -4222,7 +4220,7 @@
         <v>1.0330875719999999</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3.1496640509999998</v>
       </c>
@@ -4317,7 +4315,7 @@
         <v>2.526625514</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8.4768317900000003</v>
       </c>
@@ -4412,7 +4410,7 @@
         <v>2.8134789160000002</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2.1503743740000001</v>
       </c>
@@ -4507,7 +4505,7 @@
         <v>1.685199892</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3.199320744</v>
       </c>
@@ -4602,7 +4600,7 @@
         <v>1.827233058</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3.073316471</v>
       </c>
@@ -4697,7 +4695,7 @@
         <v>2.018697623</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5.6577042549999996</v>
       </c>
@@ -4792,7 +4790,7 @@
         <v>2.807019903</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1.8552671110000001</v>
       </c>
@@ -4887,7 +4885,7 @@
         <v>2.9401997049999999</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6.2193832999999996</v>
       </c>
@@ -4982,7 +4980,7 @@
         <v>2.7283910929999999</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1.457066864</v>
       </c>
@@ -5077,7 +5075,7 @@
         <v>2.3791588560000001</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3.8720651479999999</v>
       </c>
@@ -5172,7 +5170,7 @@
         <v>2.1568684060000001</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4.2496791189999996</v>
       </c>
@@ -5267,7 +5265,7 @@
         <v>2.0892454539999998</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5.2956371649999996</v>
       </c>
@@ -5362,7 +5360,7 @@
         <v>2.3755008769999999</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4.8775723949999996</v>
       </c>
@@ -5457,7 +5455,7 @@
         <v>1.042003528</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>7.505987459</v>
       </c>
@@ -5552,7 +5550,7 @@
         <v>1.3393168419999999</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5.5700638839999996</v>
       </c>
@@ -5647,7 +5645,7 @@
         <v>1.4937617729999999</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2.6521949779999998</v>
       </c>
@@ -5742,7 +5740,7 @@
         <v>2.615962675</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4.8056272450000002</v>
       </c>
@@ -5837,7 +5835,7 @@
         <v>1.9591760680000001</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2.0394573920000001</v>
       </c>
@@ -5932,7 +5930,7 @@
         <v>1.463561702</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>9.0434956579999994</v>
       </c>
@@ -6027,7 +6025,7 @@
         <v>2.7185746819999999</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6.3275655530000003</v>
       </c>
@@ -6122,7 +6120,7 @@
         <v>2.4981472149999999</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>9.5729682530000009</v>
       </c>
@@ -6217,7 +6215,7 @@
         <v>2.3321907369999999</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>9.7138195970000005</v>
       </c>
@@ -6312,7 +6310,7 @@
         <v>2.8482328379999999</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3.1541557409999998</v>
       </c>
@@ -6407,7 +6405,7 @@
         <v>1.909519958</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0.75838512700000005</v>
       </c>
@@ -6502,7 +6500,7 @@
         <v>1.461410232</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1.3355725540000001</v>
       </c>
@@ -6597,7 +6595,7 @@
         <v>1.296263293</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>6.13628032</v>
       </c>
@@ -6692,7 +6690,7 @@
         <v>2.8225503619999999</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4.0695782070000002</v>
       </c>
@@ -6787,7 +6785,7 @@
         <v>2.3253798589999999</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2.7805801520000002</v>
       </c>
@@ -6882,7 +6880,7 @@
         <v>2.2282915650000001</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3.363461934</v>
       </c>
@@ -6977,7 +6975,7 @@
         <v>2.019971924</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0.184739758</v>
       </c>
@@ -7072,7 +7070,7 @@
         <v>1.3126554619999999</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>5.0455600220000001</v>
       </c>
@@ -7167,7 +7165,7 @@
         <v>1.5331706430000001</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3.6435125639999999</v>
       </c>
@@ -7262,7 +7260,7 @@
         <v>1.357002735</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>9.1364504439999994</v>
       </c>
@@ -7357,7 +7355,7 @@
         <v>1.7193570869999999</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3.2249549439999998</v>
       </c>
@@ -7452,7 +7450,7 @@
         <v>1.062269245</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>4.065189438</v>
       </c>
@@ -7547,7 +7545,7 @@
         <v>1.773216916</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>5.6005174650000003</v>
       </c>
@@ -7642,7 +7640,7 @@
         <v>1.880240726</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4.6338642610000003</v>
       </c>
@@ -7737,7 +7735,7 @@
         <v>1.867603259</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3.7998510990000001</v>
       </c>
@@ -7832,7 +7830,7 @@
         <v>2.53292121</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2.6523271689999999</v>
       </c>
@@ -7927,7 +7925,7 @@
         <v>2.6864838610000001</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>5.9776249650000004</v>
       </c>
@@ -8022,7 +8020,7 @@
         <v>1.6568642659999999</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>5.4378850569999999</v>
       </c>
@@ -8117,7 +8115,7 @@
         <v>2.5857880940000002</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2.2395502490000001</v>
       </c>
@@ -8212,7 +8210,7 @@
         <v>1.384282056</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>5.9483985260000001</v>
       </c>
@@ -8307,7 +8305,7 @@
         <v>2.3972216180000001</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>6.5094367540000002</v>
       </c>
@@ -8402,7 +8400,7 @@
         <v>1.3468634049999999</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0.188713624</v>
       </c>
@@ -8497,7 +8495,7 @@
         <v>2.6126391280000001</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7.0900558910000004</v>
       </c>
@@ -8592,7 +8590,7 @@
         <v>2.0766644520000002</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>6.4079026700000004</v>
       </c>
@@ -8687,7 +8685,7 @@
         <v>2.8817951960000001</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>3.336195306</v>
       </c>
@@ -8782,7 +8780,7 @@
         <v>2.3437898580000001</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>8.8567343009999995</v>
       </c>
@@ -8877,7 +8875,7 @@
         <v>2.9900396410000001</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2.788791056</v>
       </c>
@@ -8972,7 +8970,7 @@
         <v>2.5793418680000002</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8.2939452679999999</v>
       </c>
@@ -9067,7 +9065,7 @@
         <v>1.3291437749999999</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>5.0636886839999997</v>
       </c>
@@ -9162,7 +9160,7 @@
         <v>1.024549851</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4.7386238690000004</v>
       </c>
@@ -9257,7 +9255,7 @@
         <v>1.7816536860000001</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8.1508628939999994</v>
       </c>
@@ -9352,7 +9350,7 @@
         <v>2.5716341329999999</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0.62883908899999996</v>
       </c>
@@ -9447,7 +9445,7 @@
         <v>1.6443633559999999</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3.2863320279999999</v>
       </c>
@@ -9542,7 +9540,7 @@
         <v>2.085356472</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2.0466708179999999</v>
       </c>
@@ -9637,7 +9635,7 @@
         <v>2.7889603360000002</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>3.559281661</v>
       </c>
@@ -9732,7 +9730,7 @@
         <v>1.7908478219999999</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>9.5802410550000001</v>
       </c>
@@ -9827,7 +9825,7 @@
         <v>1.545559232</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>6.0010199990000004</v>
       </c>
@@ -9922,7 +9920,7 @@
         <v>1.0102146940000001</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>7.073224851</v>
       </c>
@@ -10017,7 +10015,7 @@
         <v>1.8142555279999999</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1.9725029249999999</v>
       </c>
@@ -10112,7 +10110,7 @@
         <v>2.8754229790000001</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>6.9629868909999999</v>
       </c>
@@ -10207,7 +10205,7 @@
         <v>1.508493791</v>
       </c>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0.78244517800000002</v>
       </c>
@@ -10302,7 +10300,7 @@
         <v>1.56450248</v>
       </c>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4.1814222819999998</v>
       </c>
@@ -10397,7 +10395,7 @@
         <v>2.6456534679999999</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>3.487982514</v>
       </c>
@@ -10492,7 +10490,7 @@
         <v>1.75419788</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>5.81875666</v>
       </c>

</xml_diff>